<commit_message>
alterando caminho da planilha
</commit_message>
<xml_diff>
--- a/planilha fechamento.xlsx
+++ b/planilha fechamento.xlsx
@@ -304,7 +304,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:G36"/>
+  <dimension ref="A1:G98"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="250" zoomScaleNormal="250" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
@@ -1386,37 +1386,1987 @@
       </c>
     </row>
     <row r="36">
-      <c r="A36" t="inlineStr">
-        <is>
-          <t>Daniel da Mata</t>
-        </is>
-      </c>
-      <c r="B36" t="n">
-        <v>736.92</v>
-      </c>
-      <c r="C36" t="inlineStr">
-        <is>
-          <t>593.048.762-65</t>
-        </is>
-      </c>
-      <c r="D36" t="inlineStr">
-        <is>
-          <t>07/12/2024</t>
-        </is>
-      </c>
-      <c r="E36" t="inlineStr">
-        <is>
-          <t>em dia</t>
-        </is>
-      </c>
-      <c r="F36" t="inlineStr">
+      <c r="A36" s="4" t="inlineStr">
+        <is>
+          <t>Daniel da Mata</t>
+        </is>
+      </c>
+      <c r="B36" s="4" t="n">
+        <v>736.92</v>
+      </c>
+      <c r="C36" s="4" t="inlineStr">
+        <is>
+          <t>593.048.762-65</t>
+        </is>
+      </c>
+      <c r="D36" s="4" t="inlineStr">
+        <is>
+          <t>07/12/2024</t>
+        </is>
+      </c>
+      <c r="E36" s="4" t="inlineStr">
+        <is>
+          <t>em dia</t>
+        </is>
+      </c>
+      <c r="F36" s="4" t="inlineStr">
         <is>
           <t>01/07/2024</t>
         </is>
       </c>
-      <c r="G36" t="inlineStr">
+      <c r="G36" s="4" t="inlineStr">
         <is>
           <t>boleto</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="4" t="inlineStr">
+        <is>
+          <t>Noah da Mota</t>
+        </is>
+      </c>
+      <c r="B37" s="4" t="n">
+        <v>747.91</v>
+      </c>
+      <c r="C37" s="4" t="inlineStr">
+        <is>
+          <t>472.963.815-82</t>
+        </is>
+      </c>
+      <c r="D37" s="4" t="inlineStr">
+        <is>
+          <t>07/04/2024</t>
+        </is>
+      </c>
+      <c r="E37" s="4" t="inlineStr">
+        <is>
+          <t>em dia</t>
+        </is>
+      </c>
+      <c r="F37" s="4" t="inlineStr">
+        <is>
+          <t>14/09/2024</t>
+        </is>
+      </c>
+      <c r="G37" s="4" t="inlineStr">
+        <is>
+          <t>cartão</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="4" t="inlineStr">
+        <is>
+          <t>Noah da Mota</t>
+        </is>
+      </c>
+      <c r="B38" s="4" t="n">
+        <v>747.91</v>
+      </c>
+      <c r="C38" s="4" t="inlineStr">
+        <is>
+          <t>472.963.815-82</t>
+        </is>
+      </c>
+      <c r="D38" s="4" t="inlineStr">
+        <is>
+          <t>07/04/2024</t>
+        </is>
+      </c>
+      <c r="E38" s="4" t="inlineStr">
+        <is>
+          <t>em dia</t>
+        </is>
+      </c>
+      <c r="F38" s="4" t="inlineStr">
+        <is>
+          <t>02/07/2024</t>
+        </is>
+      </c>
+      <c r="G38" s="4" t="inlineStr">
+        <is>
+          <t>cartão</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="4" t="inlineStr">
+        <is>
+          <t>Carlos Eduardo Santos</t>
+        </is>
+      </c>
+      <c r="B39" s="4" t="n">
+        <v>123.2</v>
+      </c>
+      <c r="C39" s="4" t="inlineStr">
+        <is>
+          <t>231.659.708-40</t>
+        </is>
+      </c>
+      <c r="D39" s="4" t="inlineStr">
+        <is>
+          <t>07/12/2024</t>
+        </is>
+      </c>
+      <c r="E39" s="4" t="inlineStr">
+        <is>
+          <t>em dia</t>
+        </is>
+      </c>
+      <c r="F39" s="4" t="inlineStr">
+        <is>
+          <t>27/11/2024</t>
+        </is>
+      </c>
+      <c r="G39" s="4" t="inlineStr">
+        <is>
+          <t>cartão</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="4" t="inlineStr">
+        <is>
+          <t>Dr. Felipe Farias</t>
+        </is>
+      </c>
+      <c r="B40" s="4" t="n">
+        <v>285.56</v>
+      </c>
+      <c r="C40" s="4" t="inlineStr">
+        <is>
+          <t>487.039.126-04</t>
+        </is>
+      </c>
+      <c r="D40" s="4" t="inlineStr">
+        <is>
+          <t>07/02/2024</t>
+        </is>
+      </c>
+      <c r="E40" s="4" t="inlineStr">
+        <is>
+          <t>pendente</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="4" t="inlineStr">
+        <is>
+          <t>Luigi Barros</t>
+        </is>
+      </c>
+      <c r="B41" s="4" t="n">
+        <v>349.87</v>
+      </c>
+      <c r="C41" s="4" t="inlineStr">
+        <is>
+          <t>179.432.680-40</t>
+        </is>
+      </c>
+      <c r="D41" s="4" t="inlineStr">
+        <is>
+          <t>29/06/2024</t>
+        </is>
+      </c>
+      <c r="E41" s="4" t="inlineStr">
+        <is>
+          <t>pendente</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="4" t="inlineStr">
+        <is>
+          <t>Stella da Luz</t>
+        </is>
+      </c>
+      <c r="B42" s="4" t="n">
+        <v>449.42</v>
+      </c>
+      <c r="C42" s="4" t="inlineStr">
+        <is>
+          <t>821.074.653-71</t>
+        </is>
+      </c>
+      <c r="D42" s="4" t="inlineStr">
+        <is>
+          <t>16/07/2024</t>
+        </is>
+      </c>
+      <c r="E42" s="4" t="inlineStr">
+        <is>
+          <t>em dia</t>
+        </is>
+      </c>
+      <c r="F42" s="4" t="inlineStr">
+        <is>
+          <t>06/03/2024</t>
+        </is>
+      </c>
+      <c r="G42" s="4" t="inlineStr">
+        <is>
+          <t>boleto</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="4" t="inlineStr">
+        <is>
+          <t>Elisa da Cunha</t>
+        </is>
+      </c>
+      <c r="B43" s="4" t="n">
+        <v>655.34</v>
+      </c>
+      <c r="C43" s="4" t="inlineStr">
+        <is>
+          <t>281.597.640-49</t>
+        </is>
+      </c>
+      <c r="D43" s="4" t="inlineStr">
+        <is>
+          <t>07/05/2024</t>
+        </is>
+      </c>
+      <c r="E43" s="4" t="inlineStr">
+        <is>
+          <t>em dia</t>
+        </is>
+      </c>
+      <c r="F43" s="4" t="inlineStr">
+        <is>
+          <t>02/06/2024</t>
+        </is>
+      </c>
+      <c r="G43" s="4" t="inlineStr">
+        <is>
+          <t>cartão</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="4" t="inlineStr">
+        <is>
+          <t>Rodrigo Fernandes</t>
+        </is>
+      </c>
+      <c r="B44" s="4" t="n">
+        <v>615.39</v>
+      </c>
+      <c r="C44" s="4" t="inlineStr">
+        <is>
+          <t>358.170.962-77</t>
+        </is>
+      </c>
+      <c r="D44" s="4" t="inlineStr">
+        <is>
+          <t>13/07/2024</t>
+        </is>
+      </c>
+      <c r="E44" s="4" t="inlineStr">
+        <is>
+          <t>em dia</t>
+        </is>
+      </c>
+      <c r="F44" s="4" t="inlineStr">
+        <is>
+          <t>07/06/2024</t>
+        </is>
+      </c>
+      <c r="G44" s="4" t="inlineStr">
+        <is>
+          <t>boleto</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="4" t="inlineStr">
+        <is>
+          <t>Dra. Alícia Monteiro</t>
+        </is>
+      </c>
+      <c r="B45" s="4" t="n">
+        <v>726.4299999999999</v>
+      </c>
+      <c r="C45" s="4" t="inlineStr">
+        <is>
+          <t>098.132.475-41</t>
+        </is>
+      </c>
+      <c r="D45" s="4" t="inlineStr">
+        <is>
+          <t>26/06/2024</t>
+        </is>
+      </c>
+      <c r="E45" s="4" t="inlineStr">
+        <is>
+          <t>pendente</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="4" t="inlineStr">
+        <is>
+          <t>Eduardo Farias</t>
+        </is>
+      </c>
+      <c r="B46" s="4" t="n">
+        <v>370.38</v>
+      </c>
+      <c r="C46" s="4" t="inlineStr">
+        <is>
+          <t>203.546.178-26</t>
+        </is>
+      </c>
+      <c r="D46" s="4" t="inlineStr">
+        <is>
+          <t>23/06/2024</t>
+        </is>
+      </c>
+      <c r="E46" s="4" t="inlineStr">
+        <is>
+          <t>em dia</t>
+        </is>
+      </c>
+      <c r="F46" s="4" t="inlineStr">
+        <is>
+          <t>03/12/2024</t>
+        </is>
+      </c>
+      <c r="G46" s="4" t="inlineStr">
+        <is>
+          <t>boleto</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="4" t="inlineStr">
+        <is>
+          <t>Dr. Gustavo Costa</t>
+        </is>
+      </c>
+      <c r="B47" s="4" t="n">
+        <v>949.45</v>
+      </c>
+      <c r="C47" s="4" t="inlineStr">
+        <is>
+          <t>916.253.408-42</t>
+        </is>
+      </c>
+      <c r="D47" s="4" t="inlineStr">
+        <is>
+          <t>07/12/2024</t>
+        </is>
+      </c>
+      <c r="E47" s="4" t="inlineStr">
+        <is>
+          <t>pendente</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="4" t="inlineStr">
+        <is>
+          <t>Sarah Fogaça</t>
+        </is>
+      </c>
+      <c r="B48" s="4" t="n">
+        <v>661.26</v>
+      </c>
+      <c r="C48" s="4" t="inlineStr">
+        <is>
+          <t>197.382.460-40</t>
+        </is>
+      </c>
+      <c r="D48" s="4" t="inlineStr">
+        <is>
+          <t>27/06/2024</t>
+        </is>
+      </c>
+      <c r="E48" s="4" t="inlineStr">
+        <is>
+          <t>em dia</t>
+        </is>
+      </c>
+      <c r="F48" s="4" t="inlineStr">
+        <is>
+          <t>26/11/2024</t>
+        </is>
+      </c>
+      <c r="G48" s="4" t="inlineStr">
+        <is>
+          <t>boleto</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="4" t="inlineStr">
+        <is>
+          <t>Thomas Costa</t>
+        </is>
+      </c>
+      <c r="B49" s="4" t="n">
+        <v>375.81</v>
+      </c>
+      <c r="C49" s="4" t="inlineStr">
+        <is>
+          <t>732.481.056-07</t>
+        </is>
+      </c>
+      <c r="D49" s="4" t="inlineStr">
+        <is>
+          <t>07/06/2024</t>
+        </is>
+      </c>
+      <c r="E49" s="4" t="inlineStr">
+        <is>
+          <t>em dia</t>
+        </is>
+      </c>
+      <c r="F49" s="4" t="inlineStr">
+        <is>
+          <t>13/03/2024</t>
+        </is>
+      </c>
+      <c r="G49" s="4" t="inlineStr">
+        <is>
+          <t>boleto</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="4" t="inlineStr">
+        <is>
+          <t>João Felipe Aragão</t>
+        </is>
+      </c>
+      <c r="B50" s="4" t="n">
+        <v>666.9299999999999</v>
+      </c>
+      <c r="C50" s="4" t="inlineStr">
+        <is>
+          <t>839.140.256-89</t>
+        </is>
+      </c>
+      <c r="D50" s="4" t="inlineStr">
+        <is>
+          <t>07/08/2024</t>
+        </is>
+      </c>
+      <c r="E50" s="4" t="inlineStr">
+        <is>
+          <t>pendente</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="4" t="inlineStr">
+        <is>
+          <t>Dra. Nina Caldeira</t>
+        </is>
+      </c>
+      <c r="B51" s="4" t="n">
+        <v>618.96</v>
+      </c>
+      <c r="C51" s="4" t="inlineStr">
+        <is>
+          <t>903.158.764-84</t>
+        </is>
+      </c>
+      <c r="D51" s="4" t="inlineStr">
+        <is>
+          <t>07/12/2024</t>
+        </is>
+      </c>
+      <c r="E51" s="4" t="inlineStr">
+        <is>
+          <t>pendente</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="4" t="inlineStr">
+        <is>
+          <t>Pietra Correia</t>
+        </is>
+      </c>
+      <c r="B52" s="4" t="n">
+        <v>737.74</v>
+      </c>
+      <c r="C52" s="4" t="inlineStr">
+        <is>
+          <t>392.104.568-15</t>
+        </is>
+      </c>
+      <c r="D52" s="4" t="inlineStr">
+        <is>
+          <t>20/06/2024</t>
+        </is>
+      </c>
+      <c r="E52" s="4" t="inlineStr">
+        <is>
+          <t>em dia</t>
+        </is>
+      </c>
+      <c r="F52" s="4" t="inlineStr">
+        <is>
+          <t>27/08/2024</t>
+        </is>
+      </c>
+      <c r="G52" s="4" t="inlineStr">
+        <is>
+          <t>boleto</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="4" t="inlineStr">
+        <is>
+          <t>Enzo Gabriel Lima</t>
+        </is>
+      </c>
+      <c r="B53" s="4" t="n">
+        <v>791.46</v>
+      </c>
+      <c r="C53" s="4" t="inlineStr">
+        <is>
+          <t>185.603.294-98</t>
+        </is>
+      </c>
+      <c r="D53" s="4" t="inlineStr">
+        <is>
+          <t>07/09/2024</t>
+        </is>
+      </c>
+      <c r="E53" s="4" t="inlineStr">
+        <is>
+          <t>em dia</t>
+        </is>
+      </c>
+      <c r="F53" s="4" t="inlineStr">
+        <is>
+          <t>04/04/2024</t>
+        </is>
+      </c>
+      <c r="G53" s="4" t="inlineStr">
+        <is>
+          <t>boleto</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="4" t="inlineStr">
+        <is>
+          <t>Bianca Azevedo</t>
+        </is>
+      </c>
+      <c r="B54" s="4" t="n">
+        <v>852.28</v>
+      </c>
+      <c r="C54" s="4" t="inlineStr">
+        <is>
+          <t>143.789.560-39</t>
+        </is>
+      </c>
+      <c r="D54" s="4" t="inlineStr">
+        <is>
+          <t>24/06/2024</t>
+        </is>
+      </c>
+      <c r="E54" s="4" t="inlineStr">
+        <is>
+          <t>em dia</t>
+        </is>
+      </c>
+      <c r="F54" s="4" t="inlineStr">
+        <is>
+          <t>03/08/2024</t>
+        </is>
+      </c>
+      <c r="G54" s="4" t="inlineStr">
+        <is>
+          <t>cartão</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="4" t="inlineStr">
+        <is>
+          <t>Fernanda Martins</t>
+        </is>
+      </c>
+      <c r="B55" s="4" t="n">
+        <v>523.92</v>
+      </c>
+      <c r="C55" s="4" t="inlineStr">
+        <is>
+          <t>852.436.970-10</t>
+        </is>
+      </c>
+      <c r="D55" s="4" t="inlineStr">
+        <is>
+          <t>07/09/2024</t>
+        </is>
+      </c>
+      <c r="E55" s="4" t="inlineStr">
+        <is>
+          <t>em dia</t>
+        </is>
+      </c>
+      <c r="F55" s="4" t="inlineStr">
+        <is>
+          <t>02/10/2024</t>
+        </is>
+      </c>
+      <c r="G55" s="4" t="inlineStr">
+        <is>
+          <t>cartão</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="4" t="inlineStr">
+        <is>
+          <t>Eduardo Novaes</t>
+        </is>
+      </c>
+      <c r="B56" s="4" t="n">
+        <v>453.74</v>
+      </c>
+      <c r="C56" s="4" t="inlineStr">
+        <is>
+          <t>382.567.490-83</t>
+        </is>
+      </c>
+      <c r="D56" s="4" t="inlineStr">
+        <is>
+          <t>07/05/2024</t>
+        </is>
+      </c>
+      <c r="E56" s="4" t="inlineStr">
+        <is>
+          <t>em dia</t>
+        </is>
+      </c>
+      <c r="F56" s="4" t="inlineStr">
+        <is>
+          <t>15/08/2024</t>
+        </is>
+      </c>
+      <c r="G56" s="4" t="inlineStr">
+        <is>
+          <t>cartão</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="4" t="inlineStr">
+        <is>
+          <t>Luiz Miguel Rodrigues</t>
+        </is>
+      </c>
+      <c r="B57" s="4" t="n">
+        <v>278.83</v>
+      </c>
+      <c r="C57" s="4" t="inlineStr">
+        <is>
+          <t>903.468.752-00</t>
+        </is>
+      </c>
+      <c r="D57" s="4" t="inlineStr">
+        <is>
+          <t>21/06/2024</t>
+        </is>
+      </c>
+      <c r="E57" s="4" t="inlineStr">
+        <is>
+          <t>em dia</t>
+        </is>
+      </c>
+      <c r="F57" s="4" t="inlineStr">
+        <is>
+          <t>04/02/2024</t>
+        </is>
+      </c>
+      <c r="G57" s="4" t="inlineStr">
+        <is>
+          <t>cartão</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="4" t="inlineStr">
+        <is>
+          <t>Alexandre Ramos</t>
+        </is>
+      </c>
+      <c r="B58" s="4" t="n">
+        <v>495.02</v>
+      </c>
+      <c r="C58" s="4" t="inlineStr">
+        <is>
+          <t>370.549.268-38</t>
+        </is>
+      </c>
+      <c r="D58" s="4" t="inlineStr">
+        <is>
+          <t>07/06/2024</t>
+        </is>
+      </c>
+      <c r="E58" s="4" t="inlineStr">
+        <is>
+          <t>pendente</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="4" t="inlineStr">
+        <is>
+          <t>Danilo Peixoto</t>
+        </is>
+      </c>
+      <c r="B59" s="4" t="n">
+        <v>527.24</v>
+      </c>
+      <c r="C59" s="4" t="inlineStr">
+        <is>
+          <t>379.681.520-03</t>
+        </is>
+      </c>
+      <c r="D59" s="4" t="inlineStr">
+        <is>
+          <t>24/06/2024</t>
+        </is>
+      </c>
+      <c r="E59" s="4" t="inlineStr">
+        <is>
+          <t>pendente</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="4" t="inlineStr">
+        <is>
+          <t>Maria Eduarda Barbosa</t>
+        </is>
+      </c>
+      <c r="B60" s="4" t="n">
+        <v>164.61</v>
+      </c>
+      <c r="C60" s="4" t="inlineStr">
+        <is>
+          <t>068.719.435-01</t>
+        </is>
+      </c>
+      <c r="D60" s="4" t="inlineStr">
+        <is>
+          <t>22/06/2024</t>
+        </is>
+      </c>
+      <c r="E60" s="4" t="inlineStr">
+        <is>
+          <t>em dia</t>
+        </is>
+      </c>
+      <c r="F60" s="4" t="inlineStr">
+        <is>
+          <t>13/08/2024</t>
+        </is>
+      </c>
+      <c r="G60" s="4" t="inlineStr">
+        <is>
+          <t>boleto</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="4" t="inlineStr">
+        <is>
+          <t>Luiza Teixeira</t>
+        </is>
+      </c>
+      <c r="B61" s="4" t="n">
+        <v>236.86</v>
+      </c>
+      <c r="C61" s="4" t="inlineStr">
+        <is>
+          <t>394.275.610-25</t>
+        </is>
+      </c>
+      <c r="D61" s="4" t="inlineStr">
+        <is>
+          <t>13/07/2024</t>
+        </is>
+      </c>
+      <c r="E61" s="4" t="inlineStr">
+        <is>
+          <t>em dia</t>
+        </is>
+      </c>
+      <c r="F61" s="4" t="inlineStr">
+        <is>
+          <t>24/01/2024</t>
+        </is>
+      </c>
+      <c r="G61" s="4" t="inlineStr">
+        <is>
+          <t>cartão</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="4" t="inlineStr">
+        <is>
+          <t>Sr. Gabriel Ramos</t>
+        </is>
+      </c>
+      <c r="B62" s="4" t="n">
+        <v>942.09</v>
+      </c>
+      <c r="C62" s="4" t="inlineStr">
+        <is>
+          <t>467.831.950-66</t>
+        </is>
+      </c>
+      <c r="D62" s="4" t="inlineStr">
+        <is>
+          <t>14/07/2024</t>
+        </is>
+      </c>
+      <c r="E62" s="4" t="inlineStr">
+        <is>
+          <t>em dia</t>
+        </is>
+      </c>
+      <c r="F62" s="4" t="inlineStr">
+        <is>
+          <t>14/09/2024</t>
+        </is>
+      </c>
+      <c r="G62" s="4" t="inlineStr">
+        <is>
+          <t>boleto</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="4" t="inlineStr">
+        <is>
+          <t>Theo Oliveira</t>
+        </is>
+      </c>
+      <c r="B63" s="4" t="n">
+        <v>858.2</v>
+      </c>
+      <c r="C63" s="4" t="inlineStr">
+        <is>
+          <t>407.856.913-75</t>
+        </is>
+      </c>
+      <c r="D63" s="4" t="inlineStr">
+        <is>
+          <t>18/06/2024</t>
+        </is>
+      </c>
+      <c r="E63" s="4" t="inlineStr">
+        <is>
+          <t>pendente</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="4" t="inlineStr">
+        <is>
+          <t>Levi Caldeira</t>
+        </is>
+      </c>
+      <c r="B64" s="4" t="n">
+        <v>913.08</v>
+      </c>
+      <c r="C64" s="4" t="inlineStr">
+        <is>
+          <t>427.839.561-28</t>
+        </is>
+      </c>
+      <c r="D64" s="4" t="inlineStr">
+        <is>
+          <t>07/04/2024</t>
+        </is>
+      </c>
+      <c r="E64" s="4" t="inlineStr">
+        <is>
+          <t>pendente</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="4" t="inlineStr">
+        <is>
+          <t>Sr. Francisco Moura</t>
+        </is>
+      </c>
+      <c r="B65" s="4" t="n">
+        <v>294.91</v>
+      </c>
+      <c r="C65" s="4" t="inlineStr">
+        <is>
+          <t>912.045.687-58</t>
+        </is>
+      </c>
+      <c r="D65" s="4" t="inlineStr">
+        <is>
+          <t>16/07/2024</t>
+        </is>
+      </c>
+      <c r="E65" s="4" t="inlineStr">
+        <is>
+          <t>em dia</t>
+        </is>
+      </c>
+      <c r="F65" s="4" t="inlineStr">
+        <is>
+          <t>11/06/2024</t>
+        </is>
+      </c>
+      <c r="G65" s="4" t="inlineStr">
+        <is>
+          <t>cartão</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="4" t="inlineStr">
+        <is>
+          <t>Miguel Carvalho</t>
+        </is>
+      </c>
+      <c r="B66" s="4" t="n">
+        <v>118.37</v>
+      </c>
+      <c r="C66" s="4" t="inlineStr">
+        <is>
+          <t>497.102.653-34</t>
+        </is>
+      </c>
+      <c r="D66" s="4" t="inlineStr">
+        <is>
+          <t>16/07/2024</t>
+        </is>
+      </c>
+      <c r="E66" s="4" t="inlineStr">
+        <is>
+          <t>em dia</t>
+        </is>
+      </c>
+      <c r="F66" s="4" t="inlineStr">
+        <is>
+          <t>13/01/2024</t>
+        </is>
+      </c>
+      <c r="G66" s="4" t="inlineStr">
+        <is>
+          <t>boleto</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="4" t="inlineStr">
+        <is>
+          <t>Lorena Gomes</t>
+        </is>
+      </c>
+      <c r="B67" s="4" t="n">
+        <v>492.57</v>
+      </c>
+      <c r="C67" s="4" t="inlineStr">
+        <is>
+          <t>324.071.596-16</t>
+        </is>
+      </c>
+      <c r="D67" s="4" t="inlineStr">
+        <is>
+          <t>23/06/2024</t>
+        </is>
+      </c>
+      <c r="E67" s="4" t="inlineStr">
+        <is>
+          <t>pendente</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="4" t="inlineStr">
+        <is>
+          <t>Vitória Aragão</t>
+        </is>
+      </c>
+      <c r="B68" s="4" t="n">
+        <v>797.4400000000001</v>
+      </c>
+      <c r="C68" s="4" t="inlineStr">
+        <is>
+          <t>146.723.805-80</t>
+        </is>
+      </c>
+      <c r="D68" s="4" t="inlineStr">
+        <is>
+          <t>28/06/2024</t>
+        </is>
+      </c>
+      <c r="E68" s="4" t="inlineStr">
+        <is>
+          <t>em dia</t>
+        </is>
+      </c>
+      <c r="F68" s="4" t="inlineStr">
+        <is>
+          <t>24/06/2024</t>
+        </is>
+      </c>
+      <c r="G68" s="4" t="inlineStr">
+        <is>
+          <t>cartão</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="4" t="inlineStr">
+        <is>
+          <t>João Guilherme Costela</t>
+        </is>
+      </c>
+      <c r="B69" s="4" t="n">
+        <v>247.62</v>
+      </c>
+      <c r="C69" s="4" t="inlineStr">
+        <is>
+          <t>865.493.107-84</t>
+        </is>
+      </c>
+      <c r="D69" s="4" t="inlineStr">
+        <is>
+          <t>20/06/2024</t>
+        </is>
+      </c>
+      <c r="E69" s="4" t="inlineStr">
+        <is>
+          <t>em dia</t>
+        </is>
+      </c>
+      <c r="F69" s="4" t="inlineStr">
+        <is>
+          <t>04/03/2024</t>
+        </is>
+      </c>
+      <c r="G69" s="4" t="inlineStr">
+        <is>
+          <t>cartão</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="4" t="inlineStr">
+        <is>
+          <t>Guilherme da Rocha</t>
+        </is>
+      </c>
+      <c r="B70" s="4" t="n">
+        <v>675.64</v>
+      </c>
+      <c r="C70" s="4" t="inlineStr">
+        <is>
+          <t>921.057.386-21</t>
+        </is>
+      </c>
+      <c r="D70" s="4" t="inlineStr">
+        <is>
+          <t>21/06/2024</t>
+        </is>
+      </c>
+      <c r="E70" s="4" t="inlineStr">
+        <is>
+          <t>pendente</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="4" t="inlineStr">
+        <is>
+          <t>Raquel Nascimento</t>
+        </is>
+      </c>
+      <c r="B71" s="4" t="n">
+        <v>978.63</v>
+      </c>
+      <c r="C71" s="4" t="inlineStr">
+        <is>
+          <t>924.783.506-29</t>
+        </is>
+      </c>
+      <c r="D71" s="4" t="inlineStr">
+        <is>
+          <t>15/07/2024</t>
+        </is>
+      </c>
+      <c r="E71" s="4" t="inlineStr">
+        <is>
+          <t>em dia</t>
+        </is>
+      </c>
+      <c r="F71" s="4" t="inlineStr">
+        <is>
+          <t>06/07/2024</t>
+        </is>
+      </c>
+      <c r="G71" s="4" t="inlineStr">
+        <is>
+          <t>cartão</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="4" t="inlineStr">
+        <is>
+          <t>Mariana Carvalho</t>
+        </is>
+      </c>
+      <c r="B72" s="4" t="n">
+        <v>670.58</v>
+      </c>
+      <c r="C72" s="4" t="inlineStr">
+        <is>
+          <t>326.081.957-68</t>
+        </is>
+      </c>
+      <c r="D72" s="4" t="inlineStr">
+        <is>
+          <t>18/06/2024</t>
+        </is>
+      </c>
+      <c r="E72" s="4" t="inlineStr">
+        <is>
+          <t>em dia</t>
+        </is>
+      </c>
+      <c r="F72" s="4" t="inlineStr">
+        <is>
+          <t>06/08/2024</t>
+        </is>
+      </c>
+      <c r="G72" s="4" t="inlineStr">
+        <is>
+          <t>cartão</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="4" t="inlineStr">
+        <is>
+          <t>Laura Ramos</t>
+        </is>
+      </c>
+      <c r="B73" s="4" t="n">
+        <v>341.26</v>
+      </c>
+      <c r="C73" s="4" t="inlineStr">
+        <is>
+          <t>052.163.874-71</t>
+        </is>
+      </c>
+      <c r="D73" s="4" t="inlineStr">
+        <is>
+          <t>22/06/2024</t>
+        </is>
+      </c>
+      <c r="E73" s="4" t="inlineStr">
+        <is>
+          <t>em dia</t>
+        </is>
+      </c>
+      <c r="F73" s="4" t="inlineStr">
+        <is>
+          <t>13/04/2024</t>
+        </is>
+      </c>
+      <c r="G73" s="4" t="inlineStr">
+        <is>
+          <t>cartão</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="4" t="inlineStr">
+        <is>
+          <t>Davi da Cunha</t>
+        </is>
+      </c>
+      <c r="B74" s="4" t="n">
+        <v>510.08</v>
+      </c>
+      <c r="C74" s="4" t="inlineStr">
+        <is>
+          <t>425.068.197-11</t>
+        </is>
+      </c>
+      <c r="D74" s="4" t="inlineStr">
+        <is>
+          <t>07/08/2024</t>
+        </is>
+      </c>
+      <c r="E74" s="4" t="inlineStr">
+        <is>
+          <t>em dia</t>
+        </is>
+      </c>
+      <c r="F74" s="4" t="inlineStr">
+        <is>
+          <t>11/01/2024</t>
+        </is>
+      </c>
+      <c r="G74" s="4" t="inlineStr">
+        <is>
+          <t>cartão</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="4" t="inlineStr">
+        <is>
+          <t>Ana Beatriz Sales</t>
+        </is>
+      </c>
+      <c r="B75" s="4" t="n">
+        <v>908.97</v>
+      </c>
+      <c r="C75" s="4" t="inlineStr">
+        <is>
+          <t>694.830.271-87</t>
+        </is>
+      </c>
+      <c r="D75" s="4" t="inlineStr">
+        <is>
+          <t>07/11/2024</t>
+        </is>
+      </c>
+      <c r="E75" s="4" t="inlineStr">
+        <is>
+          <t>pendente</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="4" t="inlineStr">
+        <is>
+          <t>Melissa Silva</t>
+        </is>
+      </c>
+      <c r="B76" s="4" t="n">
+        <v>309.63</v>
+      </c>
+      <c r="C76" s="4" t="inlineStr">
+        <is>
+          <t>726.135.094-06</t>
+        </is>
+      </c>
+      <c r="D76" s="4" t="inlineStr">
+        <is>
+          <t>07/09/2024</t>
+        </is>
+      </c>
+      <c r="E76" s="4" t="inlineStr">
+        <is>
+          <t>pendente</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="4" t="inlineStr">
+        <is>
+          <t>Vitor Hugo Duarte</t>
+        </is>
+      </c>
+      <c r="B77" s="4" t="n">
+        <v>808.59</v>
+      </c>
+      <c r="C77" s="4" t="inlineStr">
+        <is>
+          <t>543.712.986-64</t>
+        </is>
+      </c>
+      <c r="D77" s="4" t="inlineStr">
+        <is>
+          <t>23/06/2024</t>
+        </is>
+      </c>
+      <c r="E77" s="4" t="inlineStr">
+        <is>
+          <t>em dia</t>
+        </is>
+      </c>
+      <c r="F77" s="4" t="inlineStr">
+        <is>
+          <t>08/05/2024</t>
+        </is>
+      </c>
+      <c r="G77" s="4" t="inlineStr">
+        <is>
+          <t>cartão</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="4" t="inlineStr">
+        <is>
+          <t>Dr. Davi Fogaça</t>
+        </is>
+      </c>
+      <c r="B78" s="4" t="n">
+        <v>560.1</v>
+      </c>
+      <c r="C78" s="4" t="inlineStr">
+        <is>
+          <t>328.105.497-88</t>
+        </is>
+      </c>
+      <c r="D78" s="4" t="inlineStr">
+        <is>
+          <t>07/04/2024</t>
+        </is>
+      </c>
+      <c r="E78" s="4" t="inlineStr">
+        <is>
+          <t>em dia</t>
+        </is>
+      </c>
+      <c r="F78" s="4" t="inlineStr">
+        <is>
+          <t>05/06/2024</t>
+        </is>
+      </c>
+      <c r="G78" s="4" t="inlineStr">
+        <is>
+          <t>cartão</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="4" t="inlineStr">
+        <is>
+          <t>Marcela Moura</t>
+        </is>
+      </c>
+      <c r="B79" s="4" t="n">
+        <v>485.08</v>
+      </c>
+      <c r="C79" s="4" t="inlineStr">
+        <is>
+          <t>790.456.218-94</t>
+        </is>
+      </c>
+      <c r="D79" s="4" t="inlineStr">
+        <is>
+          <t>07/07/2024</t>
+        </is>
+      </c>
+      <c r="E79" s="4" t="inlineStr">
+        <is>
+          <t>em dia</t>
+        </is>
+      </c>
+      <c r="F79" s="4" t="inlineStr">
+        <is>
+          <t>25/07/2024</t>
+        </is>
+      </c>
+      <c r="G79" s="4" t="inlineStr">
+        <is>
+          <t>boleto</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="4" t="inlineStr">
+        <is>
+          <t>Nina Gomes</t>
+        </is>
+      </c>
+      <c r="B80" s="4" t="n">
+        <v>853.04</v>
+      </c>
+      <c r="C80" s="4" t="inlineStr">
+        <is>
+          <t>746.298.301-03</t>
+        </is>
+      </c>
+      <c r="D80" s="4" t="inlineStr">
+        <is>
+          <t>07/03/2024</t>
+        </is>
+      </c>
+      <c r="E80" s="4" t="inlineStr">
+        <is>
+          <t>pendente</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="4" t="inlineStr">
+        <is>
+          <t>Maria Julia Dias</t>
+        </is>
+      </c>
+      <c r="B81" s="4" t="n">
+        <v>927.3200000000001</v>
+      </c>
+      <c r="C81" s="4" t="inlineStr">
+        <is>
+          <t>461.820.953-42</t>
+        </is>
+      </c>
+      <c r="D81" s="4" t="inlineStr">
+        <is>
+          <t>07/11/2024</t>
+        </is>
+      </c>
+      <c r="E81" s="4" t="inlineStr">
+        <is>
+          <t>em dia</t>
+        </is>
+      </c>
+      <c r="F81" s="4" t="inlineStr">
+        <is>
+          <t>25/03/2024</t>
+        </is>
+      </c>
+      <c r="G81" s="4" t="inlineStr">
+        <is>
+          <t>cartão</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="4" t="inlineStr">
+        <is>
+          <t>Danilo Duarte</t>
+        </is>
+      </c>
+      <c r="B82" s="4" t="n">
+        <v>836.33</v>
+      </c>
+      <c r="C82" s="4" t="inlineStr">
+        <is>
+          <t>930.126.874-40</t>
+        </is>
+      </c>
+      <c r="D82" s="4" t="inlineStr">
+        <is>
+          <t>15/07/2024</t>
+        </is>
+      </c>
+      <c r="E82" s="4" t="inlineStr">
+        <is>
+          <t>em dia</t>
+        </is>
+      </c>
+      <c r="F82" s="4" t="inlineStr">
+        <is>
+          <t>14/08/2024</t>
+        </is>
+      </c>
+      <c r="G82" s="4" t="inlineStr">
+        <is>
+          <t>boleto</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="4" t="inlineStr">
+        <is>
+          <t>Kevin Santos</t>
+        </is>
+      </c>
+      <c r="B83" s="4" t="n">
+        <v>469.74</v>
+      </c>
+      <c r="C83" s="4" t="inlineStr">
+        <is>
+          <t>107.483.259-05</t>
+        </is>
+      </c>
+      <c r="D83" s="4" t="inlineStr">
+        <is>
+          <t>18/06/2024</t>
+        </is>
+      </c>
+      <c r="E83" s="4" t="inlineStr">
+        <is>
+          <t>pendente</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="4" t="inlineStr">
+        <is>
+          <t>Rebeca Moraes</t>
+        </is>
+      </c>
+      <c r="B84" s="4" t="n">
+        <v>185.48</v>
+      </c>
+      <c r="C84" s="4" t="inlineStr">
+        <is>
+          <t>496.321.057-61</t>
+        </is>
+      </c>
+      <c r="D84" s="4" t="inlineStr">
+        <is>
+          <t>07/04/2024</t>
+        </is>
+      </c>
+      <c r="E84" s="4" t="inlineStr">
+        <is>
+          <t>em dia</t>
+        </is>
+      </c>
+      <c r="F84" s="4" t="inlineStr">
+        <is>
+          <t>03/06/2024</t>
+        </is>
+      </c>
+      <c r="G84" s="4" t="inlineStr">
+        <is>
+          <t>boleto</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="4" t="inlineStr">
+        <is>
+          <t>Enzo Costela</t>
+        </is>
+      </c>
+      <c r="B85" s="4" t="n">
+        <v>807.96</v>
+      </c>
+      <c r="C85" s="4" t="inlineStr">
+        <is>
+          <t>835.742.961-00</t>
+        </is>
+      </c>
+      <c r="D85" s="4" t="inlineStr">
+        <is>
+          <t>29/06/2024</t>
+        </is>
+      </c>
+      <c r="E85" s="4" t="inlineStr">
+        <is>
+          <t>em dia</t>
+        </is>
+      </c>
+      <c r="F85" s="4" t="inlineStr">
+        <is>
+          <t>28/03/2024</t>
+        </is>
+      </c>
+      <c r="G85" s="4" t="inlineStr">
+        <is>
+          <t>cartão</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="4" t="inlineStr">
+        <is>
+          <t>Joaquim Viana</t>
+        </is>
+      </c>
+      <c r="B86" s="4" t="n">
+        <v>992.8099999999999</v>
+      </c>
+      <c r="C86" s="4" t="inlineStr">
+        <is>
+          <t>318.742.095-88</t>
+        </is>
+      </c>
+      <c r="D86" s="4" t="inlineStr">
+        <is>
+          <t>20/06/2024</t>
+        </is>
+      </c>
+      <c r="E86" s="4" t="inlineStr">
+        <is>
+          <t>pendente</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="4" t="inlineStr">
+        <is>
+          <t>Isadora da Rosa</t>
+        </is>
+      </c>
+      <c r="B87" s="4" t="n">
+        <v>526.54</v>
+      </c>
+      <c r="C87" s="4" t="inlineStr">
+        <is>
+          <t>546.718.309-57</t>
+        </is>
+      </c>
+      <c r="D87" s="4" t="inlineStr">
+        <is>
+          <t>13/07/2024</t>
+        </is>
+      </c>
+      <c r="E87" s="4" t="inlineStr">
+        <is>
+          <t>em dia</t>
+        </is>
+      </c>
+      <c r="F87" s="4" t="inlineStr">
+        <is>
+          <t>05/09/2024</t>
+        </is>
+      </c>
+      <c r="G87" s="4" t="inlineStr">
+        <is>
+          <t>cartão</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="4" t="inlineStr">
+        <is>
+          <t>Yuri Freitas</t>
+        </is>
+      </c>
+      <c r="B88" s="4" t="n">
+        <v>725.75</v>
+      </c>
+      <c r="C88" s="4" t="inlineStr">
+        <is>
+          <t>047.298.165-01</t>
+        </is>
+      </c>
+      <c r="D88" s="4" t="inlineStr">
+        <is>
+          <t>28/06/2024</t>
+        </is>
+      </c>
+      <c r="E88" s="4" t="inlineStr">
+        <is>
+          <t>em dia</t>
+        </is>
+      </c>
+      <c r="F88" s="4" t="inlineStr">
+        <is>
+          <t>05/03/2024</t>
+        </is>
+      </c>
+      <c r="G88" s="4" t="inlineStr">
+        <is>
+          <t>boleto</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" s="4" t="inlineStr">
+        <is>
+          <t>Sabrina Pires</t>
+        </is>
+      </c>
+      <c r="B89" s="4" t="n">
+        <v>755.97</v>
+      </c>
+      <c r="C89" s="4" t="inlineStr">
+        <is>
+          <t>738.916.245-73</t>
+        </is>
+      </c>
+      <c r="D89" s="4" t="inlineStr">
+        <is>
+          <t>22/06/2024</t>
+        </is>
+      </c>
+      <c r="E89" s="4" t="inlineStr">
+        <is>
+          <t>em dia</t>
+        </is>
+      </c>
+      <c r="F89" s="4" t="inlineStr">
+        <is>
+          <t>26/03/2024</t>
+        </is>
+      </c>
+      <c r="G89" s="4" t="inlineStr">
+        <is>
+          <t>cartão</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" s="4" t="inlineStr">
+        <is>
+          <t>Julia Cunha</t>
+        </is>
+      </c>
+      <c r="B90" s="4" t="n">
+        <v>408.94</v>
+      </c>
+      <c r="C90" s="4" t="inlineStr">
+        <is>
+          <t>983.641.705-20</t>
+        </is>
+      </c>
+      <c r="D90" s="4" t="inlineStr">
+        <is>
+          <t>29/06/2024</t>
+        </is>
+      </c>
+      <c r="E90" s="4" t="inlineStr">
+        <is>
+          <t>em dia</t>
+        </is>
+      </c>
+      <c r="F90" s="4" t="inlineStr">
+        <is>
+          <t>01/02/2024</t>
+        </is>
+      </c>
+      <c r="G90" s="4" t="inlineStr">
+        <is>
+          <t>boleto</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" s="4" t="inlineStr">
+        <is>
+          <t>Dra. Maysa Souza</t>
+        </is>
+      </c>
+      <c r="B91" s="4" t="n">
+        <v>415.14</v>
+      </c>
+      <c r="C91" s="4" t="inlineStr">
+        <is>
+          <t>257.946.138-82</t>
+        </is>
+      </c>
+      <c r="D91" s="4" t="inlineStr">
+        <is>
+          <t>07/11/2024</t>
+        </is>
+      </c>
+      <c r="E91" s="4" t="inlineStr">
+        <is>
+          <t>pendente</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" s="4" t="inlineStr">
+        <is>
+          <t>Stella da Paz</t>
+        </is>
+      </c>
+      <c r="B92" s="4" t="n">
+        <v>480.36</v>
+      </c>
+      <c r="C92" s="4" t="inlineStr">
+        <is>
+          <t>105.934.768-75</t>
+        </is>
+      </c>
+      <c r="D92" s="4" t="inlineStr">
+        <is>
+          <t>07/09/2024</t>
+        </is>
+      </c>
+      <c r="E92" s="4" t="inlineStr">
+        <is>
+          <t>pendente</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" s="4" t="inlineStr">
+        <is>
+          <t>Dra. Bruna Rocha</t>
+        </is>
+      </c>
+      <c r="B93" s="4" t="n">
+        <v>763.34</v>
+      </c>
+      <c r="C93" s="4" t="inlineStr">
+        <is>
+          <t>910.645.237-06</t>
+        </is>
+      </c>
+      <c r="D93" s="4" t="inlineStr">
+        <is>
+          <t>26/06/2024</t>
+        </is>
+      </c>
+      <c r="E93" s="4" t="inlineStr">
+        <is>
+          <t>em dia</t>
+        </is>
+      </c>
+      <c r="F93" s="4" t="inlineStr">
+        <is>
+          <t>01/10/2024</t>
+        </is>
+      </c>
+      <c r="G93" s="4" t="inlineStr">
+        <is>
+          <t>cartão</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" s="4" t="inlineStr">
+        <is>
+          <t>Gustavo Silva</t>
+        </is>
+      </c>
+      <c r="B94" s="4" t="n">
+        <v>838.41</v>
+      </c>
+      <c r="C94" s="4" t="inlineStr">
+        <is>
+          <t>732.541.609-16</t>
+        </is>
+      </c>
+      <c r="D94" s="4" t="inlineStr">
+        <is>
+          <t>18/06/2024</t>
+        </is>
+      </c>
+      <c r="E94" s="4" t="inlineStr">
+        <is>
+          <t>pendente</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" s="4" t="inlineStr">
+        <is>
+          <t>Isabella Moraes</t>
+        </is>
+      </c>
+      <c r="B95" s="4" t="n">
+        <v>105.66</v>
+      </c>
+      <c r="C95" s="4" t="inlineStr">
+        <is>
+          <t>236.981.475-64</t>
+        </is>
+      </c>
+      <c r="D95" s="4" t="inlineStr">
+        <is>
+          <t>07/06/2024</t>
+        </is>
+      </c>
+      <c r="E95" s="4" t="inlineStr">
+        <is>
+          <t>pendente</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" s="4" t="inlineStr">
+        <is>
+          <t>Luiz Fernando Sales</t>
+        </is>
+      </c>
+      <c r="B96" s="4" t="n">
+        <v>820.29</v>
+      </c>
+      <c r="C96" s="4" t="inlineStr">
+        <is>
+          <t>867.504.291-49</t>
+        </is>
+      </c>
+      <c r="D96" s="4" t="inlineStr">
+        <is>
+          <t>24/06/2024</t>
+        </is>
+      </c>
+      <c r="E96" s="4" t="inlineStr">
+        <is>
+          <t>em dia</t>
+        </is>
+      </c>
+      <c r="F96" s="4" t="inlineStr">
+        <is>
+          <t>16/01/2024</t>
+        </is>
+      </c>
+      <c r="G96" s="4" t="inlineStr">
+        <is>
+          <t>cartão</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" s="4" t="inlineStr">
+        <is>
+          <t>Lavínia Costela</t>
+        </is>
+      </c>
+      <c r="B97" s="4" t="n">
+        <v>718.45</v>
+      </c>
+      <c r="C97" s="4" t="inlineStr">
+        <is>
+          <t>254.836.719-37</t>
+        </is>
+      </c>
+      <c r="D97" s="4" t="inlineStr">
+        <is>
+          <t>18/06/2024</t>
+        </is>
+      </c>
+      <c r="E97" s="4" t="inlineStr">
+        <is>
+          <t>em dia</t>
+        </is>
+      </c>
+      <c r="F97" s="4" t="inlineStr">
+        <is>
+          <t>06/09/2024</t>
+        </is>
+      </c>
+      <c r="G97" s="4" t="inlineStr">
+        <is>
+          <t>cartão</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>Dr. Juan Sales</t>
+        </is>
+      </c>
+      <c r="B98" t="n">
+        <v>301.55</v>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>463.710.892-69</t>
+        </is>
+      </c>
+      <c r="D98" t="inlineStr">
+        <is>
+          <t>23/06/2024</t>
+        </is>
+      </c>
+      <c r="E98" t="inlineStr">
+        <is>
+          <t>pendente</t>
         </is>
       </c>
     </row>

</xml_diff>